<commit_message>
Add friction coefficient calculations
</commit_message>
<xml_diff>
--- a/hardware/motor/additional_data.xlsx
+++ b/hardware/motor/additional_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Justin\School\Winter 2019\ECE 412-413\motor\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D1019F-7732-463E-8DB6-C1C089B0993F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61930170-D0C7-40A1-A851-1432BC27657E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{E4B54CB4-5D26-4052-8EAC-9BD0966E1CB3}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>